<commit_message>
Changes actually got saved this time for IO_STATE and CONTROL_MODE.
</commit_message>
<xml_diff>
--- a/Scripts/CAN/CANBusIDs.xlsx
+++ b/Scripts/CAN/CANBusIDs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madel\LHR\Embedded-Sharepoint\Scripts\CAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796D04B3-0579-4EB4-B508-CF0716CAC3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42AC2220-9AA7-45F6-BB99-3A2D9724E5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12180" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2240" yWindow="830" windowWidth="10470" windowHeight="13990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2634,7 +2634,7 @@
   </sheetPr>
   <dimension ref="A1:G1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Maybe changes saved this time?
</commit_message>
<xml_diff>
--- a/Scripts/CAN/CANBusIDs.xlsx
+++ b/Scripts/CAN/CANBusIDs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madel\LHR\Embedded-Sharepoint\Scripts\CAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42AC2220-9AA7-45F6-BB99-3A2D9724E5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074C8B3F-EF05-4781-97A8-2C5C18DFAB68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2240" yWindow="830" windowWidth="10470" windowHeight="13990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2634,7 +2634,7 @@
   </sheetPr>
   <dimension ref="A1:G1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>

</xml_diff>